<commit_message>
Updated code with dependent
</commit_message>
<xml_diff>
--- a/data/excel/FlightBooking.xlsx
+++ b/data/excel/FlightBooking.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubham.Natkar\git\Saudia\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A224DF-A50E-4B4A-BDC9-91E8312E8431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DE1141-4513-477A-ABFB-36C6FD5EF7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="124">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -392,10 +392,22 @@
     <t>ISQty</t>
   </si>
   <si>
-    <t>24-March-2025</t>
-  </si>
-  <si>
     <t>Verify one way(Dependent) flight booking flow</t>
+  </si>
+  <si>
+    <t>32 B,32 A,34 A,34 B,34 E,34 F</t>
+  </si>
+  <si>
+    <t>Baggage,Seat,MeetAndGreet,FastTrack</t>
+  </si>
+  <si>
+    <t>28-March-2025</t>
+  </si>
+  <si>
+    <t>Verify round trip(Dependent) flight booking flow</t>
+  </si>
+  <si>
+    <t>15-April-2025</t>
   </si>
 </sst>
 </file>
@@ -3983,23 +3995,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0DABC0-E5E1-486C-B0E4-ECA9269CD871}">
-  <dimension ref="A1:BF2"/>
+  <dimension ref="A1:BF3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="29.7109375" bestFit="1" customWidth="1"/>
@@ -4041,8 +4053,8 @@
     <col min="49" max="49" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="6" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="5" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="16.140625" bestFit="1" customWidth="1"/>
@@ -4231,7 +4243,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>12</v>
@@ -4270,7 +4282,7 @@
         <v>32</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="P2" s="11" t="s">
         <v>106</v>
@@ -4378,13 +4390,13 @@
         <v>3</v>
       </c>
       <c r="AY2" s="5" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="AZ2" s="5" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="BA2" s="5" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="BB2" s="5">
         <v>1</v>
@@ -4399,63 +4411,239 @@
         <v>88</v>
       </c>
       <c r="BF2">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:58" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="S3" s="5">
+        <v>2</v>
+      </c>
+      <c r="T3" s="5">
+        <v>1</v>
+      </c>
+      <c r="U3" s="5">
+        <v>1</v>
+      </c>
+      <c r="V3" s="5">
+        <v>1</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>5</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC3" s="5">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AO3" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP3" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="AQ3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AR3" s="5">
+        <v>1</v>
+      </c>
+      <c r="AS3" s="5">
+        <v>1</v>
+      </c>
+      <c r="AT3" s="5">
+        <v>1</v>
+      </c>
+      <c r="AU3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AV3" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AW3" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX3" s="5">
+        <v>3</v>
+      </c>
+      <c r="AY3" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="AZ3" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="BA3" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="BB3" s="5">
+        <v>1</v>
+      </c>
+      <c r="BC3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="BD3" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="BE3" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="BF3">
         <v>1234</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="18">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB2" xr:uid="{ADCBDE41-4393-41BD-80CC-9E1D042D15D5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB2:BB3" xr:uid="{ADCBDE41-4393-41BD-80CC-9E1D042D15D5}">
       <formula1>"1,2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BC2" xr:uid="{29BF5FF4-6162-45F7-98F1-89B6883840B8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BC2:BC3" xr:uid="{29BF5FF4-6162-45F7-98F1-89B6883840B8}">
       <formula1>"SavedCards,UseDifferentCard,SADAD"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{6B94AFED-384A-4194-9BA3-2A17C768E7E7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3" xr:uid="{6B94AFED-384A-4194-9BA3-2A17C768E7E7}">
       <formula1>"Anant Kumar,Saurabh,Prince Chaurasia,Gunjan Swain,Shubham,Laxmi Khanal,Sudesh Kumar,Piyush,Ankur,D Divaker S,Ankur Yadav,Sachin Kumar"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{EE7E1567-EF88-40F3-9405-ECD5EEC34D13}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3" xr:uid="{EE7E1567-EF88-40F3-9405-ECD5EEC34D13}">
       <formula1>"Administrator,Travel Arranger,Employee"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH2 I2" xr:uid="{45FE7830-0A38-4BFA-850C-27ED9AEC8901}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH2:AH3 I2:I3" xr:uid="{45FE7830-0A38-4BFA-850C-27ED9AEC8901}">
       <formula1>"OneWay,RoundTrip,MultiCity"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2 J2" xr:uid="{A85DB5E1-A9E3-4447-909E-DF2F07680740}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2:AI3 J2:J3" xr:uid="{A85DB5E1-A9E3-4447-909E-DF2F07680740}">
       <formula1>"Domestic,International"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2" xr:uid="{34DC906C-91D7-4FA1-B21C-84E3867758F2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q3" xr:uid="{34DC906C-91D7-4FA1-B21C-84E3867758F2}">
       <formula1>"Employee,Guest,MultiPassenger"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2 AB2" xr:uid="{84F4208B-99F5-4144-AACB-A40DD2FD649E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X3 AB2:AB3" xr:uid="{84F4208B-99F5-4144-AACB-A40DD2FD649E}">
       <formula1>"Guest,Business"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2 Z2" xr:uid="{22CE95A0-06C8-4165-A983-5DC9B830D918}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2:AD3 Z2:Z3" xr:uid="{22CE95A0-06C8-4165-A983-5DC9B830D918}">
       <formula1>"Saver,Basic,Semi Flex,Flex"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2 AE2" xr:uid="{28BCA44C-6380-4557-A5D3-48B7125820C0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2:AA3 AE2:AE3" xr:uid="{28BCA44C-6380-4557-A5D3-48B7125820C0}">
       <formula1>"Basic,Semi Flex,Flex"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2 AC2" xr:uid="{4154B67E-6035-447C-A167-520AD5CF3CDC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2:Y3 AC2:AC3" xr:uid="{4154B67E-6035-447C-A167-520AD5CF3CDC}">
       <formula1>"1,2,3,4,5,6,7,8,9,10"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2:AG2 AU2 AQ2 AN2 W2" xr:uid="{34B14E9F-6BB2-42EE-AF4D-9BEE007307B2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2:AG3 AU2:AU3 AQ2:AQ3 AN2:AN3 W2:W3" xr:uid="{34B14E9F-6BB2-42EE-AF4D-9BEE007307B2}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV2" xr:uid="{320D91A6-31ED-48DB-AAB1-B60748A35C4B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV2:AV3" xr:uid="{320D91A6-31ED-48DB-AAB1-B60748A35C4B}">
       <formula1>"Economy,Premium Economy,Business Class,First Class"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2:AT2" xr:uid="{9C60EF7A-4B43-499C-B802-40FE6C6EF111}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2:AT3" xr:uid="{9C60EF7A-4B43-499C-B802-40FE6C6EF111}">
       <formula1>"0,1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW2" xr:uid="{6BCE6FF0-2E8B-4607-82F7-972E9D989523}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW2:AW3" xr:uid="{6BCE6FF0-2E8B-4607-82F7-972E9D989523}">
       <formula1>"SelectExtras,SkipToPayment"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX2" xr:uid="{6186EBA2-615C-4AA2-9541-4FD0AD7F4B1F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX2:AX3" xr:uid="{6186EBA2-615C-4AA2-9541-4FD0AD7F4B1F}">
       <formula1>"1,2,3,4"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2" xr:uid="{17CACE01-C4D1-4582-967E-ED2725A8A2D0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R3" xr:uid="{17CACE01-C4D1-4582-967E-ED2725A8A2D0}">
       <formula1>"BusinessT,FamilyT,PersonalT"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:V2" xr:uid="{8415B70E-73A6-460E-8BB1-F70AE2DC52B8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:V3" xr:uid="{8415B70E-73A6-460E-8BB1-F70AE2DC52B8}">
       <formula1>"1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>